<commit_message>
Update Power_VRES to v0.0.3r in example
</commit_message>
<xml_diff>
--- a/data/example/Power_VRES.xlsx
+++ b/data/example/Power_VRES.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixAuer\Git\LEGO-Pyomo\InOutModule\examples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixAuer\Git\LEGO-Pyomo\data\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F23CBA6-4423-44EF-B6FA-73946D00B1FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E07FAEAC-8205-4056-A2D2-7F61C3C1417C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32565" yWindow="-21720" windowWidth="38640" windowHeight="21120" tabRatio="744" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" tabRatio="744" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="scenario" sheetId="107" r:id="rId1"/>
@@ -157,7 +157,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="78">
   <si>
     <t>[MW]</t>
   </si>
@@ -384,10 +384,13 @@
     <t>Year where it is decommissioned (31.12.xxxx)</t>
   </si>
   <si>
-    <t>v0.0.3</t>
-  </si>
-  <si>
     <t>Solar2</t>
+  </si>
+  <si>
+    <t>[°]</t>
+  </si>
+  <si>
+    <t>v0.0.3r</t>
   </si>
 </sst>
 </file>
@@ -1049,7 +1052,7 @@
         <v>29</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
@@ -1368,8 +1371,12 @@
       <c r="Q7" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="R7" s="10"/>
-      <c r="S7" s="10"/>
+      <c r="R7" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="S7" s="10" t="s">
+        <v>76</v>
+      </c>
       <c r="T7" s="10" t="s">
         <v>51</v>
       </c>
@@ -1554,7 +1561,7 @@
       <c r="A11" s="21"/>
       <c r="B11" s="22"/>
       <c r="C11" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D11" s="12" t="s">
         <v>5</v>
@@ -1684,12 +1691,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101004934E3CB1C58BA43BC6E229E2BF20201" ma:contentTypeVersion="4" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="e33ccc94e63df24f58cb47229b46e190">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87003a75-b64f-4b22-bf19-aa30740e3d46" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0f0f7a5bb162b669de9ce8ff8278c29f" ns2:_="">
     <xsd:import namespace="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
@@ -1835,6 +1836,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1845,22 +1852,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{773946F7-566C-458F-95C9-79B0CCE20E87}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1878,6 +1869,22 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Adjust Power_VRES to v0.0.4r
</commit_message>
<xml_diff>
--- a/data/example/Power_VRES.xlsx
+++ b/data/example/Power_VRES.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixAuer\Git\LEGO-Pyomo\data\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E07FAEAC-8205-4056-A2D2-7F61C3C1417C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6A6EBA0-E8A9-4522-8591-6D73C77EE380}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" tabRatio="744" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32565" yWindow="-21720" windowWidth="38640" windowHeight="21120" tabRatio="744" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="scenario" sheetId="107" r:id="rId1"/>
+    <sheet name="ScenarioA" sheetId="107" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">scenario!$C$3:$O$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ScenarioA!$C$3:$O$11</definedName>
     <definedName name="businfo">#REF!</definedName>
     <definedName name="demand">#REF!</definedName>
     <definedName name="dsmdelaytime">#REF!</definedName>
@@ -34,7 +34,7 @@
     <definedName name="inflows">#REF!</definedName>
     <definedName name="network">#REF!</definedName>
     <definedName name="param">#REF!</definedName>
-    <definedName name="renewable">scenario!$C$2:$O$643</definedName>
+    <definedName name="renewable">ScenarioA!$C$2:$O$643</definedName>
     <definedName name="resprofile">#REF!</definedName>
     <definedName name="runofriver">#REF!</definedName>
     <definedName name="sCodeName">#REF!</definedName>
@@ -157,7 +157,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="81">
   <si>
     <t>[MW]</t>
   </si>
@@ -240,9 +240,6 @@
     <t>lat</t>
   </si>
   <si>
-    <t>long</t>
-  </si>
-  <si>
     <t>Excl.</t>
   </si>
   <si>
@@ -390,7 +387,19 @@
     <t>[°]</t>
   </si>
   <si>
-    <t>v0.0.3r</t>
+    <t>v0.0.4r</t>
+  </si>
+  <si>
+    <t>excl</t>
+  </si>
+  <si>
+    <t>Commission Year</t>
+  </si>
+  <si>
+    <t>Decommission Year</t>
+  </si>
+  <si>
+    <t>lon</t>
   </si>
 </sst>
 </file>
@@ -1049,10 +1058,10 @@
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B2" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
@@ -1067,19 +1076,19 @@
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C3" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="E3" s="16" t="s">
         <v>39</v>
-      </c>
-      <c r="E3" s="16" t="s">
-        <v>40</v>
       </c>
       <c r="F3" s="16" t="s">
         <v>10</v>
@@ -1112,39 +1121,39 @@
         <v>12</v>
       </c>
       <c r="P3" s="16" t="s">
-        <v>24</v>
+        <v>78</v>
       </c>
       <c r="Q3" s="16" t="s">
-        <v>25</v>
+        <v>79</v>
       </c>
       <c r="R3" s="16" t="s">
-        <v>26</v>
+        <v>69</v>
       </c>
       <c r="S3" s="16" t="s">
-        <v>27</v>
+        <v>70</v>
       </c>
       <c r="T3" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="U3" s="16" t="s">
         <v>45</v>
-      </c>
-      <c r="U3" s="16" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
-        <v>28</v>
+        <v>77</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C4" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="E4" s="17" t="s">
         <v>36</v>
-      </c>
-      <c r="E4" s="17" t="s">
-        <v>37</v>
       </c>
       <c r="F4" s="17" t="s">
         <v>10</v>
@@ -1186,154 +1195,154 @@
         <v>26</v>
       </c>
       <c r="S4" s="17" t="s">
-        <v>27</v>
+        <v>80</v>
       </c>
       <c r="T4" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="U4" s="17" t="s">
         <v>47</v>
-      </c>
-      <c r="U4" s="17" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:24" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="18"/>
       <c r="B5" s="19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C5" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="D5" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="E5" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="E5" s="19" t="s">
+      <c r="F5" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="F5" s="19" t="s">
+      <c r="G5" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="G5" s="19" t="s">
+      <c r="H5" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="H5" s="19" t="s">
+      <c r="I5" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="I5" s="19" t="s">
+      <c r="J5" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="J5" s="19" t="s">
+      <c r="K5" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="K5" s="19" t="s">
+      <c r="L5" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="L5" s="19" t="s">
+      <c r="M5" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="M5" s="19" t="s">
+      <c r="N5" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="N5" s="19" t="s">
+      <c r="O5" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="O5" s="19" t="s">
+      <c r="P5" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q5" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="R5" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="S5" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="T5" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="P5" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q5" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="R5" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="S5" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="T5" s="19" t="s">
-        <v>69</v>
-      </c>
       <c r="U5" s="19" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="18"/>
       <c r="B6" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F6" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G6" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H6" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I6" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J6" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K6" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="L6" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="M6" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N6" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O6" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="P6" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Q6" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="R6" s="20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S6" s="20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="T6" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="U6" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
       <c r="B7" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C7" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="E7" s="10" t="s">
         <v>42</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>43</v>
       </c>
       <c r="F7" s="10" t="s">
         <v>11</v>
@@ -1354,7 +1363,7 @@
         <v>1</v>
       </c>
       <c r="L7" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M7" s="10" t="s">
         <v>16</v>
@@ -1366,22 +1375,22 @@
         <v>13</v>
       </c>
       <c r="P7" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="Q7" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="R7" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="S7" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="T7" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="U7" s="10" t="s">
         <v>51</v>
-      </c>
-      <c r="U7" s="10" t="s">
-        <v>52</v>
       </c>
       <c r="V7" s="11"/>
       <c r="W7" s="11"/>
@@ -1436,10 +1445,10 @@
         <v>12.818199999999999</v>
       </c>
       <c r="T8" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="U8" s="31" t="s">
         <v>53</v>
-      </c>
-      <c r="U8" s="31" t="s">
-        <v>54</v>
       </c>
       <c r="V8" s="8"/>
       <c r="W8" s="8"/>
@@ -1492,10 +1501,10 @@
         <v>13.746700000000001</v>
       </c>
       <c r="T9" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="U9" s="31" t="s">
         <v>53</v>
-      </c>
-      <c r="U9" s="31" t="s">
-        <v>54</v>
       </c>
       <c r="V9" s="3"/>
       <c r="W9" s="13"/>
@@ -1548,10 +1557,10 @@
         <v>13.746700000000001</v>
       </c>
       <c r="T10" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="U10" s="31" t="s">
         <v>53</v>
-      </c>
-      <c r="U10" s="31" t="s">
-        <v>54</v>
       </c>
       <c r="V10" s="3"/>
       <c r="W10" s="13"/>
@@ -1561,7 +1570,7 @@
       <c r="A11" s="21"/>
       <c r="B11" s="22"/>
       <c r="C11" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D11" s="12" t="s">
         <v>5</v>
@@ -1604,10 +1613,10 @@
         <v>14.479570000000001</v>
       </c>
       <c r="T11" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="U11" s="31" t="s">
         <v>53</v>
-      </c>
-      <c r="U11" s="31" t="s">
-        <v>54</v>
       </c>
       <c r="V11" s="3"/>
       <c r="W11" s="13"/>
@@ -1691,6 +1700,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101004934E3CB1C58BA43BC6E229E2BF20201" ma:contentTypeVersion="4" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="e33ccc94e63df24f58cb47229b46e190">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87003a75-b64f-4b22-bf19-aa30740e3d46" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0f0f7a5bb162b669de9ce8ff8278c29f" ns2:_="">
     <xsd:import namespace="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
@@ -1836,12 +1851,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1852,6 +1861,22 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{773946F7-566C-458F-95C9-79B0CCE20E87}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1869,22 +1894,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
   <ds:schemaRefs>

</xml_diff>